<commit_message>
Added code to a bunch of scripts
</commit_message>
<xml_diff>
--- a/2.Data/EnvironmentalData.xlsx
+++ b/2.Data/EnvironmentalData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/evert_sprockel_wur_nl/Documents/5.Wageningen/7.Thesis/7.DataAnalysis/ThesisRAnalysis/2.Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="439" documentId="11_38AE230EADFB0BBDC981F51D93740FD6917D560E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{324A90DD-9D0D-4C07-A165-4ADAD1BD0711}"/>
+  <xr:revisionPtr revIDLastSave="446" documentId="11_38AE230EADFB0BBDC981F51D93740FD6917D560E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3274617-3536-47D5-80AE-A148136BEA5C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>sunny</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>5Y4/1</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>S1T1P2</t>
   </si>
   <si>
-    <t>thufur</t>
-  </si>
-  <si>
     <t>2.5Y5/6;2.5Y3/3</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t>S1T1P3</t>
   </si>
   <si>
-    <t>hollow</t>
-  </si>
-  <si>
     <t>10YR5/6</t>
   </si>
   <si>
@@ -778,6 +769,15 @@
   </si>
   <si>
     <t>Contrast</t>
+  </si>
+  <si>
+    <t>Thufur</t>
+  </si>
+  <si>
+    <t>Hollow</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -788,11 +788,18 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss\ \U\T\C"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -857,47 +864,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1125,11 +1123,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1181,61 +1179,61 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="U1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>6</v>
@@ -1303,13 +1301,13 @@
         <v>4</v>
       </c>
       <c r="U2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="W2" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X2" s="2">
         <v>1</v>
@@ -1318,12 +1316,12 @@
         <v>0</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>45524</v>
@@ -1383,13 +1381,13 @@
         <v>3</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X3" s="2">
         <v>0</v>
@@ -1400,7 +1398,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3">
         <v>45524</v>
@@ -1460,13 +1458,13 @@
         <v>5</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="X4" s="2">
         <v>0</v>
@@ -1477,7 +1475,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3">
         <v>45524</v>
@@ -1492,7 +1490,7 @@
         <v>78.014341000000002</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G5" s="2">
         <v>0.36745040000000001</v>
@@ -1537,13 +1535,13 @@
         <v>5</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X5" s="2">
         <v>0</v>
@@ -1554,7 +1552,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>45524</v>
@@ -1569,7 +1567,7 @@
         <v>78.014529999999993</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G6" s="2">
         <v>0.3773705</v>
@@ -1614,13 +1612,13 @@
         <v>3</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X6" s="2">
         <v>1</v>
@@ -1629,12 +1627,12 @@
         <v>0</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3">
         <v>45524</v>
@@ -1694,13 +1692,13 @@
         <v>3</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X7" s="2">
         <v>0</v>
@@ -1709,12 +1707,12 @@
         <v>0</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3">
         <v>45524</v>
@@ -1774,13 +1772,13 @@
         <v>6</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X8" s="2">
         <v>0</v>
@@ -1791,7 +1789,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" s="3">
         <v>45524</v>
@@ -1851,13 +1849,13 @@
         <v>4</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X9" s="2">
         <v>0</v>
@@ -1866,12 +1864,12 @@
         <v>0</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B10" s="3">
         <v>45524</v>
@@ -1931,13 +1929,13 @@
         <v>2</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X10" s="2">
         <v>0</v>
@@ -1946,12 +1944,12 @@
         <v>0</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11" s="3">
         <v>45524</v>
@@ -2011,13 +2009,13 @@
         <v>2</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X11" s="2">
         <v>0</v>
@@ -2028,7 +2026,7 @@
     </row>
     <row r="12" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12" s="14">
         <v>45524</v>
@@ -2077,13 +2075,13 @@
         <v>2</v>
       </c>
       <c r="U12" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="V12" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W12" s="13" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X12" s="13">
         <v>0</v>
@@ -2092,12 +2090,12 @@
         <v>0</v>
       </c>
       <c r="Z12" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B13" s="3">
         <v>45524</v>
@@ -2157,13 +2155,13 @@
         <v>3</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X13" s="2">
         <v>0</v>
@@ -2172,12 +2170,12 @@
         <v>0</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3">
         <v>45525</v>
@@ -2237,13 +2235,13 @@
         <v>5</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X14" s="2">
         <v>0</v>
@@ -2254,7 +2252,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B15" s="3">
         <v>45525</v>
@@ -2314,13 +2312,13 @@
         <v>5</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X15" s="2">
         <v>0</v>
@@ -2329,12 +2327,12 @@
         <v>0</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B16" s="3">
         <v>45525</v>
@@ -2394,13 +2392,13 @@
         <v>3</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X16" s="2">
         <v>0</v>
@@ -2411,7 +2409,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B17" s="3">
         <v>45525</v>
@@ -2471,13 +2469,13 @@
         <v>3</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X17" s="2">
         <v>0</v>
@@ -2488,7 +2486,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B18" s="3">
         <v>45525</v>
@@ -2548,13 +2546,13 @@
         <v>4</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X18" s="2">
         <v>0</v>
@@ -2563,12 +2561,12 @@
         <v>1</v>
       </c>
       <c r="Z18" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B19" s="3">
         <v>45525</v>
@@ -2628,13 +2626,13 @@
         <v>4</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X19" s="2">
         <v>0</v>
@@ -2645,7 +2643,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B20" s="3">
         <v>45525</v>
@@ -2660,7 +2658,7 @@
         <v>78.012595000000005</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G20" s="2">
         <v>0.4592444</v>
@@ -2705,13 +2703,13 @@
         <v>5</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X20" s="2">
         <v>0</v>
@@ -2722,7 +2720,7 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B21" s="3">
         <v>45525</v>
@@ -2737,7 +2735,7 @@
         <v>78.012463999999994</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G21" s="2">
         <v>0.43910270000000001</v>
@@ -2782,13 +2780,13 @@
         <v>5</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X21" s="2">
         <v>0</v>
@@ -2799,7 +2797,7 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B22" s="3">
         <v>45525</v>
@@ -2814,7 +2812,7 @@
         <v>78.012235000000004</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G22" s="2">
         <v>0.37114009999999997</v>
@@ -2859,13 +2857,13 @@
         <v>5</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X22" s="2">
         <v>0</v>
@@ -2874,12 +2872,12 @@
         <v>0</v>
       </c>
       <c r="Z22" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B23" s="3">
         <v>45525</v>
@@ -2939,13 +2937,13 @@
         <v>5</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X23" s="2">
         <v>0</v>
@@ -2954,12 +2952,12 @@
         <v>1</v>
       </c>
       <c r="Z23" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B24" s="3">
         <v>45525</v>
@@ -2974,7 +2972,7 @@
         <v>78.011589000000001</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G24" s="2">
         <v>0.38502189999999997</v>
@@ -3019,13 +3017,13 @@
         <v>4</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X24" s="2">
         <v>0</v>
@@ -3034,12 +3032,12 @@
         <v>1</v>
       </c>
       <c r="Z24" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B25" s="3">
         <v>45525</v>
@@ -3054,7 +3052,7 @@
         <v>78.011266000000006</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G25" s="2">
         <v>0.34487250000000003</v>
@@ -3099,13 +3097,13 @@
         <v>5</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X25" s="2">
         <v>0</v>
@@ -3114,12 +3112,12 @@
         <v>0</v>
       </c>
       <c r="Z25" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B26" s="3">
         <v>45525</v>
@@ -3134,7 +3132,7 @@
         <v>78.017741999999998</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G26" s="2">
         <v>0.38738250000000002</v>
@@ -3179,13 +3177,13 @@
         <v>3</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X26" s="2">
         <v>0</v>
@@ -3196,7 +3194,7 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B27" s="3">
         <v>45525</v>
@@ -3256,13 +3254,13 @@
         <v>4</v>
       </c>
       <c r="U27" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X27" s="2">
         <v>0</v>
@@ -3273,7 +3271,7 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B28" s="3">
         <v>45525</v>
@@ -3288,7 +3286,7 @@
         <v>78.017326999999995</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G28" s="2">
         <v>0.40806890000000001</v>
@@ -3333,13 +3331,13 @@
         <v>2</v>
       </c>
       <c r="U28" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X28" s="2">
         <v>0</v>
@@ -3350,7 +3348,7 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B29" s="3">
         <v>45525</v>
@@ -3365,7 +3363,7 @@
         <v>78.016858999999997</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G29" s="2">
         <v>0.34937820000000003</v>
@@ -3410,13 +3408,13 @@
         <v>5</v>
       </c>
       <c r="U29" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="V29" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W29" s="2" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="X29" s="2">
         <v>1</v>
@@ -3425,12 +3423,12 @@
         <v>0</v>
       </c>
       <c r="Z29" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B30" s="3">
         <v>45526</v>
@@ -3490,13 +3488,13 @@
         <v>3</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W30" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X30" s="2">
         <v>1</v>
@@ -3505,12 +3503,12 @@
         <v>0</v>
       </c>
       <c r="Z30" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B31" s="3">
         <v>45526</v>
@@ -3570,13 +3568,13 @@
         <v>5</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W31" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X31" s="2">
         <v>0</v>
@@ -3587,7 +3585,7 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B32" s="3">
         <v>45526</v>
@@ -3641,13 +3639,13 @@
         <v>3</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X32" s="2">
         <v>1</v>
@@ -3656,12 +3654,12 @@
         <v>1</v>
       </c>
       <c r="Z32" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B33" s="3">
         <v>45526</v>
@@ -3721,13 +3719,13 @@
         <v>2</v>
       </c>
       <c r="U33" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W33" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X33" s="2">
         <v>0</v>
@@ -3736,12 +3734,12 @@
         <v>0</v>
       </c>
       <c r="Z33" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B34" s="3">
         <v>45526</v>
@@ -3801,13 +3799,13 @@
         <v>3</v>
       </c>
       <c r="U34" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="V34" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W34" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X34" s="2">
         <v>0</v>
@@ -3816,12 +3814,12 @@
         <v>1</v>
       </c>
       <c r="Z34" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B35" s="3">
         <v>45526</v>
@@ -3881,13 +3879,13 @@
         <v>5</v>
       </c>
       <c r="U35" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W35" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X35" s="2">
         <v>0</v>
@@ -3898,7 +3896,7 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B36" s="3">
         <v>45526</v>
@@ -3958,13 +3956,13 @@
         <v>4</v>
       </c>
       <c r="U36" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W36" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X36" s="2">
         <v>0</v>
@@ -3973,12 +3971,12 @@
         <v>0</v>
       </c>
       <c r="Z36" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B37" s="3">
         <v>45526</v>
@@ -4038,13 +4036,13 @@
         <v>5</v>
       </c>
       <c r="U37" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W37" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X37" s="2">
         <v>0</v>
@@ -4053,12 +4051,12 @@
         <v>0</v>
       </c>
       <c r="Z37" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B38" s="3">
         <v>45526</v>
@@ -4118,13 +4116,13 @@
         <v>2</v>
       </c>
       <c r="U38" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X38" s="2">
         <v>0</v>
@@ -4133,12 +4131,12 @@
         <v>1</v>
       </c>
       <c r="Z38" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B39" s="3">
         <v>45526</v>
@@ -4198,13 +4196,13 @@
         <v>3</v>
       </c>
       <c r="U39" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="V39" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W39" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X39" s="2">
         <v>0</v>
@@ -4213,12 +4211,12 @@
         <v>0</v>
       </c>
       <c r="Z39" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B40" s="3">
         <v>45526</v>
@@ -4278,13 +4276,13 @@
         <v>3</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="V40" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X40" s="2">
         <v>0</v>
@@ -4295,7 +4293,7 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B41" s="3">
         <v>45526</v>
@@ -4355,13 +4353,13 @@
         <v>3</v>
       </c>
       <c r="U41" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="V41" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W41" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X41" s="2">
         <v>0</v>
@@ -4372,7 +4370,7 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B42" s="3">
         <v>45526</v>
@@ -4432,13 +4430,13 @@
         <v>4</v>
       </c>
       <c r="U42" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W42" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X42" s="2">
         <v>0</v>
@@ -4447,12 +4445,12 @@
         <v>1</v>
       </c>
       <c r="Z42" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B43" s="3">
         <v>45526</v>
@@ -4467,7 +4465,7 @@
         <v>78.034763999999996</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G43" s="2">
         <v>0.3845964</v>
@@ -4512,13 +4510,13 @@
         <v>5</v>
       </c>
       <c r="U43" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="V43" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W43" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X43" s="2">
         <v>0</v>
@@ -4527,12 +4525,12 @@
         <v>0</v>
       </c>
       <c r="Z43" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B44" s="3">
         <v>45526</v>
@@ -4547,7 +4545,7 @@
         <v>78.038731999999996</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G44" s="2">
         <v>0.46868300000000002</v>
@@ -4592,13 +4590,13 @@
         <v>5</v>
       </c>
       <c r="U44" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="V44" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W44" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X44" s="2">
         <v>0</v>
@@ -4609,7 +4607,7 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B45" s="3">
         <v>45526</v>
@@ -4624,7 +4622,7 @@
         <v>73.038055</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G45" s="2">
         <v>0.43202689999999999</v>
@@ -4669,13 +4667,13 @@
         <v>5</v>
       </c>
       <c r="U45" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="V45" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="W45" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X45" s="2">
         <v>0</v>
@@ -4686,7 +4684,7 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B46" s="3">
         <v>45526</v>
@@ -4746,13 +4744,13 @@
         <v>3</v>
       </c>
       <c r="U46" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="V46" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W46" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X46" s="2">
         <v>0</v>
@@ -4763,7 +4761,7 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B47" s="3">
         <v>45534</v>
@@ -4778,7 +4776,7 @@
         <v>78.037305000000003</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G47" s="2">
         <v>0.44528329999999999</v>
@@ -4823,13 +4821,13 @@
         <v>3</v>
       </c>
       <c r="U47" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="V47" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W47" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X47" s="2">
         <v>0</v>
@@ -4840,7 +4838,7 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B48" s="3">
         <v>45534</v>
@@ -4855,7 +4853,7 @@
         <v>78.036923999999999</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G48" s="2">
         <v>0.34134009999999998</v>
@@ -4900,13 +4898,13 @@
         <v>7</v>
       </c>
       <c r="U48" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="V48" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W48" s="2" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="X48" s="2">
         <v>0</v>
@@ -4915,12 +4913,12 @@
         <v>1</v>
       </c>
       <c r="Z48" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B49" s="3">
         <v>45534</v>
@@ -4980,13 +4978,13 @@
         <v>5</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="V49" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W49" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X49" s="2">
         <v>0</v>
@@ -4997,7 +4995,7 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B50" s="3">
         <v>45534</v>
@@ -5057,13 +5055,13 @@
         <v>7</v>
       </c>
       <c r="U50" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="V50" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W50" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X50" s="2">
         <v>0</v>
@@ -5072,12 +5070,12 @@
         <v>0</v>
       </c>
       <c r="Z50" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B51" s="3">
         <v>45534</v>
@@ -5137,13 +5135,13 @@
         <v>6</v>
       </c>
       <c r="U51" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="V51" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="W51" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X51" s="2">
         <v>0</v>
@@ -5154,7 +5152,7 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B52" s="3">
         <v>45534</v>
@@ -5214,13 +5212,13 @@
         <v>5</v>
       </c>
       <c r="U52" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V52" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W52" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X52" s="2">
         <v>0</v>
@@ -5231,7 +5229,7 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B53" s="3">
         <v>45534</v>
@@ -5246,7 +5244,7 @@
         <v>78.036608999999999</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G53" s="2">
         <v>0.40565830000000003</v>
@@ -5291,13 +5289,13 @@
         <v>6</v>
       </c>
       <c r="U53" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V53" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W53" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X53" s="2">
         <v>0</v>
@@ -5308,7 +5306,7 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B54" s="3">
         <v>45534</v>
@@ -5323,7 +5321,7 @@
         <v>78.036979000000002</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G54" s="2">
         <v>0.3657514</v>
@@ -5368,13 +5366,13 @@
         <v>6</v>
       </c>
       <c r="U54" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="V54" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W54" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X54" s="2">
         <v>0</v>
@@ -5383,12 +5381,12 @@
         <v>0</v>
       </c>
       <c r="Z54" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:26" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B55" s="14">
         <v>45534</v>
@@ -5448,13 +5446,13 @@
         <v>5</v>
       </c>
       <c r="U55" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="V55" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W55" s="13" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="X55" s="13">
         <v>1</v>
@@ -5463,12 +5461,12 @@
         <v>0</v>
       </c>
       <c r="Z55" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B56" s="3">
         <v>45534</v>
@@ -5483,7 +5481,7 @@
         <v>78.038932000000003</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G56" s="2">
         <v>0.42669780000000002</v>
@@ -5528,13 +5526,13 @@
         <v>4</v>
       </c>
       <c r="U56" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="V56" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W56" s="2" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="X56" s="2">
         <v>0</v>
@@ -5545,7 +5543,7 @@
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B57" s="3">
         <v>45534</v>
@@ -5560,7 +5558,7 @@
         <v>78.038629</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G57" s="2">
         <v>0.40291830000000001</v>
@@ -5605,13 +5603,13 @@
         <v>2</v>
       </c>
       <c r="U57" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V57" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W57" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X57" s="2">
         <v>1</v>
@@ -5620,12 +5618,12 @@
         <v>1</v>
       </c>
       <c r="Z57" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B58" s="3">
         <v>45534</v>
@@ -5640,7 +5638,7 @@
         <v>78.038336999999999</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G58" s="2">
         <v>0.39139800000000002</v>
@@ -5685,13 +5683,13 @@
         <v>4</v>
       </c>
       <c r="U58" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="V58" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W58" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X58" s="2">
         <v>0</v>
@@ -5702,7 +5700,7 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B59" s="3">
         <v>45534</v>
@@ -5762,13 +5760,13 @@
         <v>4</v>
       </c>
       <c r="U59" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="V59" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W59" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X59" s="2">
         <v>0</v>
@@ -5777,12 +5775,12 @@
         <v>0</v>
       </c>
       <c r="Z59" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B60" s="3">
         <v>45534</v>
@@ -5842,13 +5840,13 @@
         <v>6</v>
       </c>
       <c r="U60" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="V60" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="W60" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X60" s="2">
         <v>0</v>
@@ -5859,7 +5857,7 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B61" s="3">
         <v>45534</v>
@@ -5874,7 +5872,7 @@
         <v>78.035404999999997</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G61" s="2">
         <v>0.34031519999999998</v>
@@ -5919,13 +5917,13 @@
         <v>6</v>
       </c>
       <c r="U61" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="V61" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="W61" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X61" s="2">
         <v>0</v>
@@ -5936,7 +5934,7 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B62" s="3">
         <v>45535</v>
@@ -5996,13 +5994,13 @@
         <v>6</v>
       </c>
       <c r="U62" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V62" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W62" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X62" s="2">
         <v>0</v>
@@ -6013,7 +6011,7 @@
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B63" s="3">
         <v>45535</v>
@@ -6073,13 +6071,13 @@
         <v>5</v>
       </c>
       <c r="U63" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="V63" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W63" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X63" s="2">
         <v>0</v>
@@ -6090,7 +6088,7 @@
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B64" s="3">
         <v>45535</v>
@@ -6105,7 +6103,7 @@
         <v>78.059225999999995</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G64" s="2">
         <v>0.37471589999999999</v>
@@ -6150,13 +6148,13 @@
         <v>7</v>
       </c>
       <c r="U64" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="V64" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W64" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X64" s="2">
         <v>0</v>
@@ -6167,7 +6165,7 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B65" s="3">
         <v>45535</v>
@@ -6182,7 +6180,7 @@
         <v>78.059031000000004</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G65" s="2">
         <v>0.34128740000000002</v>
@@ -6227,13 +6225,13 @@
         <v>6</v>
       </c>
       <c r="U65" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="V65" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W65" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X65" s="2">
         <v>0</v>
@@ -6242,12 +6240,12 @@
         <v>0</v>
       </c>
       <c r="Z65" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B66" s="3">
         <v>45535</v>
@@ -6307,13 +6305,13 @@
         <v>7</v>
       </c>
       <c r="U66" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="V66" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W66" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X66" s="2">
         <v>1</v>
@@ -6322,12 +6320,12 @@
         <v>0</v>
       </c>
       <c r="Z66" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B67" s="3">
         <v>45535</v>
@@ -6342,7 +6340,7 @@
         <v>78.058368000000002</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G67" s="2">
         <v>0.38143379999999999</v>
@@ -6385,13 +6383,13 @@
       </c>
       <c r="T67" s="10"/>
       <c r="U67" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="V67" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W67" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X67" s="2">
         <v>1</v>
@@ -6400,12 +6398,12 @@
         <v>0</v>
       </c>
       <c r="Z67" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B68" s="3">
         <v>45535</v>
@@ -6465,13 +6463,13 @@
         <v>5</v>
       </c>
       <c r="U68" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="V68" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W68" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X68" s="2">
         <v>1</v>
@@ -6480,12 +6478,12 @@
         <v>0</v>
       </c>
       <c r="Z68" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B69" s="3">
         <v>45535</v>
@@ -6545,13 +6543,13 @@
         <v>6</v>
       </c>
       <c r="U69" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="V69" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W69" s="2" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="X69" s="2">
         <v>0</v>
@@ -6562,7 +6560,7 @@
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B70" s="3">
         <v>45535</v>
@@ -6622,13 +6620,13 @@
         <v>5</v>
       </c>
       <c r="U70" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="V70" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W70" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X70" s="2">
         <v>0</v>
@@ -6637,12 +6635,12 @@
         <v>0</v>
       </c>
       <c r="Z70" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B71" s="3">
         <v>45535</v>
@@ -6657,7 +6655,7 @@
         <v>78.059190000000001</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G71" s="2">
         <v>0.35153489999999998</v>
@@ -6702,13 +6700,13 @@
         <v>5</v>
       </c>
       <c r="U71" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="V71" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W71" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X71" s="2">
         <v>0</v>
@@ -6719,7 +6717,7 @@
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B72" s="3">
         <v>45535</v>
@@ -6734,7 +6732,7 @@
         <v>78.058739000000003</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G72" s="2">
         <v>0.40604040000000002</v>
@@ -6779,13 +6777,13 @@
         <v>7</v>
       </c>
       <c r="U72" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="V72" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W72" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X72" s="2">
         <v>0</v>
@@ -6796,7 +6794,7 @@
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B73" s="3">
         <v>45535</v>
@@ -6850,13 +6848,13 @@
         <v>3</v>
       </c>
       <c r="U73" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="V73" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W73" s="2" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="X73" s="2">
         <v>1</v>
@@ -6865,12 +6863,12 @@
         <v>0</v>
       </c>
       <c r="Z73" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B74" s="3">
         <v>45535</v>
@@ -6885,7 +6883,7 @@
         <v>78.057182999999995</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G74" s="2">
         <v>0.35008889999999998</v>
@@ -6930,13 +6928,13 @@
         <v>7</v>
       </c>
       <c r="U74" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="V74" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W74" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X74" s="2">
         <v>0</v>
@@ -6947,7 +6945,7 @@
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B75" s="3">
         <v>45535</v>
@@ -7007,13 +7005,13 @@
         <v>6</v>
       </c>
       <c r="U75" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="V75" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W75" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X75" s="2">
         <v>0</v>
@@ -7024,7 +7022,7 @@
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B76" s="3">
         <v>45535</v>
@@ -7084,13 +7082,13 @@
         <v>5</v>
       </c>
       <c r="U76" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="V76" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W76" s="2" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="X76" s="2">
         <v>0</v>
@@ -7101,7 +7099,7 @@
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B77" s="3">
         <v>45535</v>
@@ -7116,7 +7114,7 @@
         <v>78.056336999999999</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G77" s="2">
         <v>0.34017740000000002</v>
@@ -7161,13 +7159,13 @@
         <v>7</v>
       </c>
       <c r="U77" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="V77" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W77" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X77" s="2">
         <v>0</v>
@@ -7176,12 +7174,12 @@
         <v>0</v>
       </c>
       <c r="Z77" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B78" s="3">
         <v>45535</v>
@@ -7196,7 +7194,7 @@
         <v>78.055856000000006</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G78" s="2">
         <v>0.40275100000000003</v>
@@ -7241,13 +7239,13 @@
         <v>5</v>
       </c>
       <c r="U78" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="V78" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W78" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X78" s="2">
         <v>0</v>
@@ -7256,12 +7254,12 @@
         <v>0</v>
       </c>
       <c r="Z78" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B79" s="3">
         <v>45535</v>
@@ -7276,7 +7274,7 @@
         <v>78.055674999999994</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G79" s="2">
         <v>0.41446480000000002</v>
@@ -7321,13 +7319,13 @@
         <v>5</v>
       </c>
       <c r="U79" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="V79" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W79" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X79" s="2">
         <v>0</v>
@@ -7336,12 +7334,12 @@
         <v>0</v>
       </c>
       <c r="Z79" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B80" s="3">
         <v>45536</v>
@@ -7401,13 +7399,13 @@
         <v>2</v>
       </c>
       <c r="U80" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="V80" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W80" s="2" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="X80" s="2">
         <v>0</v>
@@ -7418,7 +7416,7 @@
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B81" s="3">
         <v>45536</v>
@@ -7433,7 +7431,7 @@
         <v>78.052369999999996</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G81" s="2">
         <v>0.35297139999999999</v>
@@ -7478,13 +7476,13 @@
         <v>6</v>
       </c>
       <c r="U81" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="V81" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W81" s="2" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="X81" s="2">
         <v>0</v>
@@ -7495,7 +7493,7 @@
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B82" s="3">
         <v>45536</v>
@@ -7555,13 +7553,13 @@
         <v>4</v>
       </c>
       <c r="U82" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V82" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W82" s="2" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="X82" s="2">
         <v>0</v>
@@ -7572,7 +7570,7 @@
     </row>
     <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B83" s="3">
         <v>45536</v>
@@ -7587,7 +7585,7 @@
         <v>78.052009999999996</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G83" s="2">
         <v>0.42228559999999998</v>
@@ -7632,13 +7630,13 @@
         <v>3</v>
       </c>
       <c r="U83" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="V83" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W83" s="2" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="X83" s="2">
         <v>1</v>
@@ -7647,12 +7645,12 @@
         <v>0</v>
       </c>
       <c r="Z83" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B84" s="3">
         <v>45536</v>
@@ -7712,13 +7710,13 @@
         <v>5</v>
       </c>
       <c r="U84" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V84" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W84" s="2" t="s">
-        <v>19</v>
+        <v>245</v>
       </c>
       <c r="X84" s="2">
         <v>0</v>
@@ -7729,7 +7727,7 @@
     </row>
     <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B85" s="3">
         <v>45536</v>
@@ -7789,13 +7787,13 @@
         <v>5</v>
       </c>
       <c r="U85" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V85" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W85" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X85" s="2">
         <v>0</v>
@@ -7806,7 +7804,7 @@
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B86" s="3">
         <v>45536</v>
@@ -7866,13 +7864,13 @@
         <v>6</v>
       </c>
       <c r="U86" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="V86" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W86" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X86" s="2">
         <v>0</v>
@@ -7881,12 +7879,12 @@
         <v>0</v>
       </c>
       <c r="Z86" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B87" s="3">
         <v>45536</v>
@@ -7946,13 +7944,13 @@
         <v>5</v>
       </c>
       <c r="U87" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="V87" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W87" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X87" s="2">
         <v>0</v>
@@ -7963,7 +7961,7 @@
     </row>
     <row r="88" spans="1:26" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B88" s="14">
         <v>45536</v>
@@ -8023,13 +8021,13 @@
         <v>6</v>
       </c>
       <c r="U88" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="V88" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W88" s="13" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X88" s="13">
         <v>0</v>
@@ -8040,7 +8038,7 @@
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B89" s="3">
         <v>45536</v>
@@ -8100,13 +8098,13 @@
         <v>5</v>
       </c>
       <c r="U89" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V89" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W89" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X89" s="2">
         <v>0</v>
@@ -8117,7 +8115,7 @@
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B90" s="3">
         <v>45536</v>
@@ -8177,13 +8175,13 @@
         <v>6</v>
       </c>
       <c r="U90" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="V90" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W90" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X90" s="2">
         <v>0</v>
@@ -8194,7 +8192,7 @@
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B91" s="3">
         <v>45536</v>
@@ -8254,13 +8252,13 @@
         <v>6</v>
       </c>
       <c r="U91" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="V91" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="W91" s="2" t="s">
-        <v>10</v>
+        <v>246</v>
       </c>
       <c r="X91" s="2">
         <v>0</v>
@@ -11932,8 +11930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E773609-CAD2-4136-82CC-F9EF7F6894D9}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11945,16 +11943,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -11962,7 +11960,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -11988,7 +11986,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -11998,7 +11996,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -12008,56 +12006,56 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -12065,143 +12063,143 @@
         <v>7</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C13" t="s">
-        <v>215</v>
+        <v>222</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C14" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>227</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>233</v>
-      </c>
       <c r="D17" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D21" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C22" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>